<commit_message>
add SnpEff to the list of VEPs
</commit_message>
<xml_diff>
--- a/data/Supplementary_Table_3_list_of_included_publications.xlsx
+++ b/data/Supplementary_Table_3_list_of_included_publications.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="1087">
   <si>
     <t xml:space="preserve">List of publications included in this systematic review. The table lists the PubMed ID, tool name, publication title, journal, year of publication, creation date of the PubMed entry. SO terms related to variation types are listed alphabetically and separated by semicolons under the “variant” column. Similarly, SO terms related to predicted functional impacts are listed under the “impact” column.</t>
   </si>
@@ -2337,6 +2337,36 @@
   </si>
   <si>
     <t xml:space="preserve">10.1093/bib/bbac014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SnpEff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_prime_UTR_truncation;3_prime_UTR_variant;5_prime_UTR_premature_start_codon_gain_variant;5_prime_UTR_truncation;5_prime_UTR_variant;CDS_variant;chromosome_number_variation;coding_sequence_variant;coding_sequence_variant;conservative_inframe_deletion;conservative_inframe_insertion;conserved_intergenic_variant;conserved_intron_variant;disruptive_inframe_deletion;disruptive_inframe_insertion;downstream_gene_variant;exon_loss;exon_loss_variant;exon_loss_variant;exon_variant;feature_elongation;feature_truncation;frameshift_variant;gene_variant;initiator_codon_variant;intergenic_variant;intragenic_variant;intron_variant;mature_miRNA_variant;miRNA;missense_variant;NMD_transcript_variant;non_coding_transcript_exon_variant;non_coding_transcript_variant;nonsynonymous_variant;rare_amino_acid_variant;regulatory_region_ablation;regulatory_region_amplification;regulatory_region_variant;splice_acceptor_variant;splice_donor_variant;splice_region_variant;splice_region_variant;splice_site_variant;start_gained;start_lost;start_retained;stop_gained;stop_lost;stop_retained_variant;synonymous_variant;TF_binding_site_variant;TFBS_ablation;TFBS_amplification;transcript_ablation;transcript_amplification;transcript_variant;upstream_gene_variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A program for annotating and predicting the effects of single nucleotide polymorphisms, SnpEff: SNPs in the genome of Drosophila melanogaster strain w1118; iso-2; iso-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cingolani P, Platts A, Wang le L, Coon M, Nguyen T, Wang L, Land SJ, Lu X, Ruden DM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly (Austin). 2012 Apr-Jun;6(2):80-92. doi: 10.4161/fly.19695.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cingolani P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly (Austin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/06/2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMC3679285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.4161/fly.19695</t>
   </si>
   <si>
     <t xml:space="preserve">SparkINFERNO</t>
@@ -3291,7 +3321,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:O119" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:O120" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="15">
     <tableColumn id="1" name="PMID"/>
     <tableColumn id="2" name="Tool name"/>
@@ -7553,13 +7583,13 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>32330239</v>
+        <v>22728672</v>
       </c>
       <c r="B86" t="s">
         <v>775</v>
       </c>
       <c r="C86" t="s">
-        <v>50</v>
+        <v>557</v>
       </c>
       <c r="D86" t="s">
         <v>776</v>
@@ -7580,174 +7610,174 @@
         <v>780</v>
       </c>
       <c r="J86" t="s">
-        <v>24</v>
+        <v>781</v>
       </c>
       <c r="K86" t="n">
-        <v>2020</v>
+        <v>2012</v>
       </c>
       <c r="L86" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="M86" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="N86" t="s">
         <v>19</v>
       </c>
       <c r="O86" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>37021934</v>
+        <v>32330239</v>
       </c>
       <c r="B87" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C87" t="s">
         <v>50</v>
       </c>
       <c r="D87" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
       </c>
       <c r="F87" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="G87" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="H87" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="I87" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="J87" t="s">
         <v>24</v>
       </c>
       <c r="K87" t="n">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="L87" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="M87" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="N87" t="s">
         <v>19</v>
       </c>
       <c r="O87" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>35801945</v>
+        <v>37021934</v>
       </c>
       <c r="B88" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C88" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D88" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
       </c>
       <c r="F88" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="G88" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="H88" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="I88" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="J88" t="s">
         <v>24</v>
       </c>
       <c r="K88" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="L88" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="M88" t="s">
-        <v>19</v>
+        <v>801</v>
       </c>
       <c r="N88" t="s">
         <v>19</v>
       </c>
       <c r="O88" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>35032432</v>
+        <v>35801945</v>
       </c>
       <c r="B89" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C89" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D89" t="s">
-        <v>18</v>
+        <v>804</v>
       </c>
       <c r="E89" t="s">
         <v>19</v>
       </c>
       <c r="F89" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="G89" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="H89" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="I89" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="J89" t="s">
-        <v>174</v>
+        <v>24</v>
       </c>
       <c r="K89" t="n">
         <v>2022</v>
       </c>
       <c r="L89" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="M89" t="s">
-        <v>807</v>
+        <v>19</v>
       </c>
       <c r="N89" t="s">
         <v>19</v>
       </c>
       <c r="O89" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>35232478</v>
+        <v>35032432</v>
       </c>
       <c r="B90" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="C90" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D90" t="s">
         <v>18</v>
@@ -7756,72 +7786,72 @@
         <v>19</v>
       </c>
       <c r="F90" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="G90" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="H90" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="I90" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="J90" t="s">
-        <v>417</v>
+        <v>174</v>
       </c>
       <c r="K90" t="n">
         <v>2022</v>
       </c>
       <c r="L90" t="s">
-        <v>327</v>
+        <v>816</v>
       </c>
       <c r="M90" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="N90" t="s">
         <v>19</v>
       </c>
       <c r="O90" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>36707993</v>
+        <v>35232478</v>
       </c>
       <c r="B91" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c r="C91" t="s">
-        <v>817</v>
+        <v>94</v>
       </c>
       <c r="D91" t="s">
-        <v>818</v>
+        <v>18</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
       </c>
       <c r="F91" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="G91" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="H91" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="I91" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="J91" t="s">
-        <v>24</v>
+        <v>417</v>
       </c>
       <c r="K91" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="L91" t="s">
-        <v>823</v>
+        <v>327</v>
       </c>
       <c r="M91" t="s">
         <v>824</v>
@@ -7835,7 +7865,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>34648033</v>
+        <v>36707993</v>
       </c>
       <c r="B92" t="s">
         <v>826</v>
@@ -7844,119 +7874,119 @@
         <v>827</v>
       </c>
       <c r="D92" t="s">
-        <v>18</v>
+        <v>828</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
       </c>
       <c r="F92" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="G92" t="s">
-        <v>650</v>
+        <v>830</v>
       </c>
       <c r="H92" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="I92" t="s">
-        <v>652</v>
+        <v>832</v>
       </c>
       <c r="J92" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="K92" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="L92" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="M92" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="N92" t="s">
         <v>19</v>
       </c>
       <c r="O92" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>36063453</v>
+        <v>34648033</v>
       </c>
       <c r="B93" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="C93" t="s">
-        <v>377</v>
+        <v>837</v>
       </c>
       <c r="D93" t="s">
-        <v>367</v>
+        <v>18</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
       </c>
       <c r="F93" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="G93" t="s">
-        <v>835</v>
+        <v>650</v>
       </c>
       <c r="H93" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="I93" t="s">
-        <v>43</v>
+        <v>652</v>
       </c>
       <c r="J93" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="K93" t="n">
         <v>2022</v>
       </c>
       <c r="L93" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="M93" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="N93" t="s">
         <v>19</v>
       </c>
       <c r="O93" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>36509753</v>
+        <v>36063453</v>
       </c>
       <c r="B94" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="C94" t="s">
-        <v>29</v>
+        <v>377</v>
       </c>
       <c r="D94" t="s">
-        <v>841</v>
+        <v>367</v>
       </c>
       <c r="E94" t="s">
         <v>19</v>
       </c>
       <c r="F94" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="G94" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="H94" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="I94" t="s">
-        <v>845</v>
+        <v>43</v>
       </c>
       <c r="J94" t="s">
-        <v>846</v>
+        <v>24</v>
       </c>
       <c r="K94" t="n">
         <v>2022</v>
@@ -7976,131 +8006,131 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>34182919</v>
+        <v>36509753</v>
       </c>
       <c r="B95" t="s">
         <v>850</v>
       </c>
       <c r="C95" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D95" t="s">
-        <v>423</v>
+        <v>851</v>
       </c>
       <c r="E95" t="s">
         <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="G95" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="H95" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="I95" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="J95" t="s">
-        <v>194</v>
+        <v>856</v>
       </c>
       <c r="K95" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="L95" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="M95" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="N95" t="s">
         <v>19</v>
       </c>
       <c r="O95" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>26740527</v>
+        <v>34182919</v>
       </c>
       <c r="B96" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C96" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D96" t="s">
-        <v>859</v>
+        <v>423</v>
       </c>
       <c r="E96" t="s">
         <v>19</v>
       </c>
       <c r="F96" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="G96" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H96" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="I96" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="J96" t="s">
-        <v>24</v>
+        <v>194</v>
       </c>
       <c r="K96" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="L96" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="M96" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="N96" t="s">
         <v>19</v>
       </c>
       <c r="O96" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>30305743</v>
+        <v>26740527</v>
       </c>
       <c r="B97" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C97" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D97" t="s">
-        <v>423</v>
+        <v>869</v>
       </c>
       <c r="E97" t="s">
-        <v>868</v>
+        <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="G97" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="H97" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="I97" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="J97" t="s">
-        <v>873</v>
+        <v>24</v>
       </c>
       <c r="K97" t="n">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="L97" t="s">
         <v>874</v>
@@ -8117,131 +8147,131 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>32926138</v>
+        <v>30305743</v>
       </c>
       <c r="B98" t="s">
         <v>877</v>
       </c>
       <c r="C98" t="s">
+        <v>50</v>
+      </c>
+      <c r="D98" t="s">
+        <v>423</v>
+      </c>
+      <c r="E98" t="s">
         <v>878</v>
       </c>
-      <c r="D98" t="s">
+      <c r="F98" t="s">
         <v>879</v>
       </c>
-      <c r="E98" t="s">
+      <c r="G98" t="s">
         <v>880</v>
       </c>
-      <c r="F98" t="s">
+      <c r="H98" t="s">
         <v>881</v>
       </c>
-      <c r="G98" t="s">
+      <c r="I98" t="s">
         <v>882</v>
       </c>
-      <c r="H98" t="s">
+      <c r="J98" t="s">
         <v>883</v>
       </c>
-      <c r="I98" t="s">
+      <c r="K98" t="n">
+        <v>2018</v>
+      </c>
+      <c r="L98" t="s">
         <v>884</v>
       </c>
-      <c r="J98" t="s">
-        <v>24</v>
-      </c>
-      <c r="K98" t="n">
-        <v>2021</v>
-      </c>
-      <c r="L98" t="s">
+      <c r="M98" t="s">
         <v>885</v>
       </c>
-      <c r="M98" t="s">
+      <c r="N98" t="s">
+        <v>19</v>
+      </c>
+      <c r="O98" t="s">
         <v>886</v>
-      </c>
-      <c r="N98" t="s">
-        <v>887</v>
-      </c>
-      <c r="O98" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>30840782</v>
+        <v>32926138</v>
       </c>
       <c r="B99" t="s">
+        <v>887</v>
+      </c>
+      <c r="C99" t="s">
+        <v>888</v>
+      </c>
+      <c r="D99" t="s">
         <v>889</v>
       </c>
-      <c r="C99" t="s">
-        <v>17</v>
-      </c>
-      <c r="D99" t="s">
-        <v>18</v>
-      </c>
       <c r="E99" t="s">
-        <v>19</v>
+        <v>890</v>
       </c>
       <c r="F99" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="G99" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="H99" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="I99" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="J99" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="K99" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="L99" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="M99" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="N99" t="s">
-        <v>19</v>
+        <v>897</v>
       </c>
       <c r="O99" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>26678383</v>
+        <v>30840782</v>
       </c>
       <c r="B100" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="C100" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D100" t="s">
-        <v>898</v>
+        <v>18</v>
       </c>
       <c r="E100" t="s">
         <v>19</v>
       </c>
       <c r="F100" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="G100" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="H100" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="I100" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="J100" t="s">
-        <v>903</v>
+        <v>35</v>
       </c>
       <c r="K100" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="L100" t="s">
         <v>904</v>
@@ -8250,45 +8280,45 @@
         <v>905</v>
       </c>
       <c r="N100" t="s">
+        <v>19</v>
+      </c>
+      <c r="O100" t="s">
         <v>906</v>
-      </c>
-      <c r="O100" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>33095866</v>
+        <v>26678383</v>
       </c>
       <c r="B101" t="s">
+        <v>907</v>
+      </c>
+      <c r="C101" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" t="s">
         <v>908</v>
       </c>
-      <c r="C101" t="s">
-        <v>366</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
         <v>909</v>
       </c>
-      <c r="E101" t="s">
-        <v>19</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="G101" t="s">
         <v>910</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H101" t="s">
         <v>911</v>
       </c>
-      <c r="H101" t="s">
+      <c r="I101" t="s">
         <v>912</v>
       </c>
-      <c r="I101" t="s">
+      <c r="J101" t="s">
         <v>913</v>
       </c>
-      <c r="J101" t="s">
-        <v>56</v>
-      </c>
       <c r="K101" t="n">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="L101" t="s">
         <v>914</v>
@@ -8297,139 +8327,139 @@
         <v>915</v>
       </c>
       <c r="N101" t="s">
-        <v>19</v>
+        <v>916</v>
       </c>
       <c r="O101" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>31765830</v>
+        <v>33095866</v>
       </c>
       <c r="B102" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C102" t="s">
-        <v>50</v>
+        <v>366</v>
       </c>
       <c r="D102" t="s">
-        <v>18</v>
+        <v>919</v>
       </c>
       <c r="E102" t="s">
         <v>19</v>
       </c>
       <c r="F102" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="G102" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="H102" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="I102" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="J102" t="s">
-        <v>608</v>
+        <v>56</v>
       </c>
       <c r="K102" t="n">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="L102" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="M102" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="N102" t="s">
         <v>19</v>
       </c>
       <c r="O102" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>31317185</v>
+        <v>31765830</v>
       </c>
       <c r="B103" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C103" t="s">
         <v>50</v>
       </c>
       <c r="D103" t="s">
-        <v>926</v>
+        <v>18</v>
       </c>
       <c r="E103" t="s">
         <v>19</v>
       </c>
       <c r="F103" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="G103" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="H103" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="I103" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="J103" t="s">
-        <v>590</v>
+        <v>608</v>
       </c>
       <c r="K103" t="n">
         <v>2019</v>
       </c>
       <c r="L103" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="M103" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="N103" t="s">
         <v>19</v>
       </c>
       <c r="O103" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>26395054</v>
+        <v>31317185</v>
       </c>
       <c r="B104" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C104" t="s">
-        <v>557</v>
+        <v>50</v>
       </c>
       <c r="D104" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
       </c>
       <c r="F104" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="G104" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="H104" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="I104" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="J104" t="s">
-        <v>940</v>
+        <v>590</v>
       </c>
       <c r="K104" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="L104" t="s">
         <v>941</v>
@@ -8438,24 +8468,24 @@
         <v>942</v>
       </c>
       <c r="N104" t="s">
+        <v>19</v>
+      </c>
+      <c r="O104" t="s">
         <v>943</v>
-      </c>
-      <c r="O104" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>34407882</v>
+        <v>26395054</v>
       </c>
       <c r="B105" t="s">
+        <v>944</v>
+      </c>
+      <c r="C105" t="s">
+        <v>557</v>
+      </c>
+      <c r="D105" t="s">
         <v>945</v>
-      </c>
-      <c r="C105" t="s">
-        <v>94</v>
-      </c>
-      <c r="D105" t="s">
-        <v>18</v>
       </c>
       <c r="E105" t="s">
         <v>19</v>
@@ -8473,33 +8503,33 @@
         <v>949</v>
       </c>
       <c r="J105" t="s">
-        <v>126</v>
+        <v>950</v>
       </c>
       <c r="K105" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="L105" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="M105" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="N105" t="s">
-        <v>19</v>
+        <v>953</v>
       </c>
       <c r="O105" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>36789265</v>
+        <v>34407882</v>
       </c>
       <c r="B106" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="C106" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D106" t="s">
         <v>18</v>
@@ -8508,42 +8538,42 @@
         <v>19</v>
       </c>
       <c r="F106" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="G106" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="H106" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="I106" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="J106" t="s">
-        <v>635</v>
+        <v>126</v>
       </c>
       <c r="K106" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="L106" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="M106" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="N106" t="s">
         <v>19</v>
       </c>
       <c r="O106" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>32938008</v>
+        <v>36789265</v>
       </c>
       <c r="B107" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="C107" t="s">
         <v>86</v>
@@ -8555,48 +8585,48 @@
         <v>19</v>
       </c>
       <c r="F107" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="G107" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="H107" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="I107" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="J107" t="s">
-        <v>290</v>
+        <v>635</v>
       </c>
       <c r="K107" t="n">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="L107" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="M107" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="N107" t="s">
         <v>19</v>
       </c>
       <c r="O107" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>33261662</v>
+        <v>32938008</v>
       </c>
       <c r="B108" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C108" t="s">
-        <v>970</v>
+        <v>86</v>
       </c>
       <c r="D108" t="s">
-        <v>971</v>
+        <v>18</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
@@ -8611,69 +8641,69 @@
         <v>974</v>
       </c>
       <c r="I108" t="s">
-        <v>939</v>
+        <v>975</v>
       </c>
       <c r="J108" t="s">
-        <v>126</v>
+        <v>290</v>
       </c>
       <c r="K108" t="n">
         <v>2020</v>
       </c>
       <c r="L108" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="M108" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="N108" t="s">
         <v>19</v>
       </c>
       <c r="O108" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>26075791</v>
+        <v>33261662</v>
       </c>
       <c r="B109" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C109" t="s">
-        <v>50</v>
+        <v>980</v>
       </c>
       <c r="D109" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E109" t="s">
         <v>19</v>
       </c>
       <c r="F109" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="G109" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="H109" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="I109" t="s">
-        <v>983</v>
+        <v>949</v>
       </c>
       <c r="J109" t="s">
-        <v>268</v>
+        <v>126</v>
       </c>
       <c r="K109" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="L109" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="M109" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="N109" t="s">
-        <v>986</v>
+        <v>19</v>
       </c>
       <c r="O109" t="s">
         <v>987</v>
@@ -8681,16 +8711,16 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>34859531</v>
+        <v>26075791</v>
       </c>
       <c r="B110" t="s">
         <v>988</v>
       </c>
       <c r="C110" t="s">
+        <v>50</v>
+      </c>
+      <c r="D110" t="s">
         <v>989</v>
-      </c>
-      <c r="D110" t="s">
-        <v>423</v>
       </c>
       <c r="E110" t="s">
         <v>19</v>
@@ -8708,10 +8738,10 @@
         <v>993</v>
       </c>
       <c r="J110" t="s">
-        <v>35</v>
+        <v>268</v>
       </c>
       <c r="K110" t="n">
-        <v>2022</v>
+        <v>2015</v>
       </c>
       <c r="L110" t="s">
         <v>994</v>
@@ -8728,7 +8758,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>33686085</v>
+        <v>34859531</v>
       </c>
       <c r="B111" t="s">
         <v>998</v>
@@ -8737,7 +8767,7 @@
         <v>999</v>
       </c>
       <c r="D111" t="s">
-        <v>18</v>
+        <v>423</v>
       </c>
       <c r="E111" t="s">
         <v>19</v>
@@ -8755,10 +8785,10 @@
         <v>1003</v>
       </c>
       <c r="J111" t="s">
-        <v>372</v>
+        <v>35</v>
       </c>
       <c r="K111" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="L111" t="s">
         <v>1004</v>
@@ -8767,92 +8797,92 @@
         <v>1005</v>
       </c>
       <c r="N111" t="s">
-        <v>19</v>
+        <v>1006</v>
       </c>
       <c r="O111" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>29036329</v>
+        <v>33686085</v>
       </c>
       <c r="B112" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C112" t="s">
-        <v>50</v>
+        <v>1009</v>
       </c>
       <c r="D112" t="s">
-        <v>1008</v>
+        <v>18</v>
       </c>
       <c r="E112" t="s">
         <v>19</v>
       </c>
       <c r="F112" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="G112" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="H112" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I112" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="J112" t="s">
-        <v>56</v>
+        <v>372</v>
       </c>
       <c r="K112" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="L112" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="M112" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="N112" t="s">
         <v>19</v>
       </c>
       <c r="O112" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>33407088</v>
+        <v>29036329</v>
       </c>
       <c r="B113" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C113" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D113" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="E113" t="s">
         <v>19</v>
       </c>
       <c r="F113" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="G113" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="H113" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="I113" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="J113" t="s">
-        <v>1022</v>
+        <v>56</v>
       </c>
       <c r="K113" t="n">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="L113" t="s">
         <v>1023</v>
@@ -8869,60 +8899,60 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>33258967</v>
+        <v>33407088</v>
       </c>
       <c r="B114" t="s">
         <v>1026</v>
       </c>
       <c r="C114" t="s">
-        <v>377</v>
+        <v>78</v>
       </c>
       <c r="D114" t="s">
-        <v>18</v>
+        <v>1027</v>
       </c>
       <c r="E114" t="s">
         <v>19</v>
       </c>
       <c r="F114" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="G114" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="H114" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I114" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="J114" t="s">
-        <v>590</v>
+        <v>1032</v>
       </c>
       <c r="K114" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="L114" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="M114" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="N114" t="s">
         <v>19</v>
       </c>
       <c r="O114" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>32444882</v>
+        <v>33258967</v>
       </c>
       <c r="B115" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C115" t="s">
-        <v>50</v>
+        <v>377</v>
       </c>
       <c r="D115" t="s">
         <v>18</v>
@@ -8931,139 +8961,139 @@
         <v>19</v>
       </c>
       <c r="F115" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="G115" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="H115" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="I115" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="J115" t="s">
-        <v>644</v>
+        <v>590</v>
       </c>
       <c r="K115" t="n">
         <v>2020</v>
       </c>
       <c r="L115" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="M115" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="N115" t="s">
         <v>19</v>
       </c>
       <c r="O115" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>32461655</v>
+        <v>32444882</v>
       </c>
       <c r="B116" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C116" t="s">
         <v>50</v>
       </c>
       <c r="D116" t="s">
-        <v>1043</v>
+        <v>18</v>
       </c>
       <c r="E116" t="s">
         <v>19</v>
       </c>
       <c r="F116" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="G116" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="H116" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="I116" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="J116" t="s">
-        <v>873</v>
+        <v>644</v>
       </c>
       <c r="K116" t="n">
         <v>2020</v>
       </c>
       <c r="L116" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="M116" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="N116" t="s">
         <v>19</v>
       </c>
       <c r="O116" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>36611253</v>
+        <v>32461655</v>
       </c>
       <c r="B117" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C117" t="s">
-        <v>1052</v>
+        <v>50</v>
       </c>
       <c r="D117" t="s">
-        <v>18</v>
+        <v>1053</v>
       </c>
       <c r="E117" t="s">
         <v>19</v>
       </c>
       <c r="F117" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="G117" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="H117" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="I117" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="J117" t="s">
-        <v>772</v>
+        <v>883</v>
       </c>
       <c r="K117" t="n">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="L117" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="M117" t="s">
-        <v>19</v>
+        <v>1059</v>
       </c>
       <c r="N117" t="s">
         <v>19</v>
       </c>
       <c r="O117" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>36651276</v>
+        <v>36611253</v>
       </c>
       <c r="B118" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="C118" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="D118" t="s">
         <v>18</v>
@@ -9072,81 +9102,128 @@
         <v>19</v>
       </c>
       <c r="F118" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="G118" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="H118" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="I118" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="J118" t="s">
-        <v>56</v>
+        <v>772</v>
       </c>
       <c r="K118" t="n">
         <v>2023</v>
       </c>
       <c r="L118" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="M118" t="s">
-        <v>1066</v>
+        <v>19</v>
       </c>
       <c r="N118" t="s">
         <v>19</v>
       </c>
       <c r="O118" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
+        <v>36651276</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D119" t="s">
+        <v>18</v>
+      </c>
+      <c r="E119" t="s">
+        <v>19</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G119" t="s">
+        <v>1072</v>
+      </c>
+      <c r="H119" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I119" t="s">
+        <v>1074</v>
+      </c>
+      <c r="J119" t="s">
+        <v>56</v>
+      </c>
+      <c r="K119" t="n">
+        <v>2023</v>
+      </c>
+      <c r="L119" t="s">
+        <v>1075</v>
+      </c>
+      <c r="M119" t="s">
+        <v>1076</v>
+      </c>
+      <c r="N119" t="s">
+        <v>19</v>
+      </c>
+      <c r="O119" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
         <v>34478494</v>
       </c>
-      <c r="B119" t="s">
-        <v>1068</v>
-      </c>
-      <c r="C119" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="B120" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D120" t="s">
         <v>603</v>
       </c>
-      <c r="E119" t="s">
-        <v>19</v>
-      </c>
-      <c r="F119" t="s">
-        <v>1070</v>
-      </c>
-      <c r="G119" t="s">
-        <v>1071</v>
-      </c>
-      <c r="H119" t="s">
-        <v>1072</v>
-      </c>
-      <c r="I119" t="s">
-        <v>1073</v>
-      </c>
-      <c r="J119" t="s">
+      <c r="E120" t="s">
+        <v>19</v>
+      </c>
+      <c r="F120" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G120" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H120" t="s">
+        <v>1082</v>
+      </c>
+      <c r="I120" t="s">
+        <v>1083</v>
+      </c>
+      <c r="J120" t="s">
         <v>24</v>
       </c>
-      <c r="K119" t="n">
+      <c r="K120" t="n">
         <v>2021</v>
       </c>
-      <c r="L119" t="s">
-        <v>1074</v>
-      </c>
-      <c r="M119" t="s">
-        <v>1075</v>
-      </c>
-      <c r="N119" t="s">
-        <v>19</v>
-      </c>
-      <c r="O119" t="s">
-        <v>1076</v>
+      <c r="L120" t="s">
+        <v>1084</v>
+      </c>
+      <c r="M120" t="s">
+        <v>1085</v>
+      </c>
+      <c r="N120" t="s">
+        <v>19</v>
+      </c>
+      <c r="O120" t="s">
+        <v>1086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>